<commit_message>
edit error data null in file excel
</commit_message>
<xml_diff>
--- a/TiLeTotNghiep.xlsx
+++ b/TiLeTotNghiep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binhm\Desktop\Luan_An\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7391F033-9209-430C-9039-6A39D9D97FED}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{56305282-84BE-4B83-89E6-3E1C2513C56B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="360" windowWidth="17955" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
show mess all list school not have tiledo
</commit_message>
<xml_diff>
--- a/TiLeTotNghiep.xlsx
+++ b/TiLeTotNghiep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binhm\Desktop\Luan_An\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8C30232E-FF90-48A6-8D06-C90FCBA00001}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{60694F81-4438-439D-A8D8-B0EEB33F469C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="360" windowWidth="17955" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>VHD</t>
   </si>
   <si>
-    <t>TiLe</t>
-  </si>
-  <si>
     <t>XDA</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>VUI</t>
+  </si>
+  <si>
+    <t>TiLeDo</t>
   </si>
 </sst>
 </file>
@@ -820,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,12 +836,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3">
         <v>89.95</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="3">
         <v>86.69</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3">
         <v>88.85</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3">
         <v>81.58</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38" s="3">
         <v>82.55</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3">
         <v>80</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3">
         <v>85.75</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="3">
         <v>88.56</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3">
         <v>80.56</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="3">
         <v>78.5</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" s="3">
         <v>81.25</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" s="3">
         <v>85</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" s="3">
         <v>75.849999999999994</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47" s="3">
         <v>88</v>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" s="3">
         <v>78.849999999999994</v>
@@ -1217,7 +1217,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="3">
         <v>77.5</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" s="3">
         <v>81</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" s="3">
         <v>82.56</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="3">
         <v>80.5</v>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" s="3">
         <v>83.5</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="3">
         <v>84.5</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3">
         <v>82.58</v>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" s="3">
         <v>87</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" s="3">
         <v>83.86</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="3">
         <v>81</v>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="3">
         <v>84.55</v>
@@ -1305,7 +1305,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" s="3">
         <v>87.85</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" s="3">
         <v>78.98</v>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" s="3">
         <v>83.51</v>
@@ -1329,7 +1329,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3">
         <v>85.98</v>
@@ -1337,7 +1337,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" s="3">
         <v>85.75</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3">
         <v>81</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="3">
         <v>81.56</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" s="3">
         <v>86.76</v>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="3">
         <v>85.74</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" s="3">
         <v>83.58</v>
@@ -1385,7 +1385,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" s="3">
         <v>88.3</v>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" s="3">
         <v>82</v>
@@ -1401,7 +1401,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" s="3">
         <v>82.33</v>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" s="3">
         <v>80.3</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" s="3">
         <v>84.3</v>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3">
         <v>83.3</v>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" s="3">
         <v>82.28</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="3">
         <v>88</v>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="3">
         <v>89.83</v>
@@ -1457,7 +1457,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B79" s="3">
         <v>88</v>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B80" s="3">
         <v>88.33</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B81" s="3">
         <v>88.93</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" s="3">
         <v>89.98</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" s="3">
         <v>84.3</v>
@@ -1497,7 +1497,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B84" s="3">
         <v>83.98</v>
@@ -1505,7 +1505,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85" s="3">
         <v>88.83</v>
@@ -1513,7 +1513,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B86" s="3">
         <v>80</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B87" s="3">
         <v>82.33</v>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B88" s="3">
         <v>83.83</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B89" s="3">
         <v>82.84</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B90" s="3">
         <v>83.39</v>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B91" s="3">
         <v>88.83</v>
@@ -1561,7 +1561,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B92" s="3">
         <v>82.38</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" s="3">
         <v>82.33</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B94" s="3">
         <v>80</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" s="3">
         <v>83.83</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" s="3">
         <v>88.33</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" s="3">
         <v>80.33</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B98" s="3">
         <v>88.3</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B99" s="3">
         <v>82.23</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B100" s="3">
         <v>83</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B101" s="3">
         <v>83.83</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B102" s="3">
         <v>88</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B103" s="3">
         <v>88.83</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B104" s="3">
         <v>88.3</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B105" s="3">
         <v>82</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B106" s="3">
         <v>82.33</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" s="3">
         <v>80.3</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B108" s="3">
         <v>83.3</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B109" s="3">
         <v>84.3</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B110" s="3">
         <v>82.38</v>
@@ -1713,7 +1713,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B111" s="3">
         <v>88</v>
@@ -1721,7 +1721,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B112" s="3">
         <v>83.83</v>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B113" s="3">
         <v>82</v>
@@ -1737,7 +1737,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B114" s="3">
         <v>84.33</v>
@@ -1745,7 +1745,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B115" s="3">
         <v>88.83</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B116" s="3">
         <v>88.98</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B117" s="3">
         <v>83.32</v>
@@ -1769,7 +1769,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B118" s="3">
         <v>83.98</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B119" s="3">
         <v>83.83</v>
@@ -1785,7 +1785,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B120" s="3">
         <v>82</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B121" s="3">
         <v>82.33</v>
@@ -1801,7 +1801,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B122" s="3">
         <v>83.83</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B123" s="3">
         <v>83.84</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B124" s="3">
         <v>83.38</v>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B125" s="3">
         <v>85</v>
@@ -1833,7 +1833,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B126" s="3">
         <v>83.66</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B127" s="3">
         <v>88.86</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B128" s="3">
         <v>88.98</v>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B129" s="3">
         <v>86.62</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B130" s="3">
         <v>86.98</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B131" s="3">
         <v>86.86</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B132" s="3">
         <v>82</v>
@@ -1889,7 +1889,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B133" s="3">
         <v>82.66</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B134" s="3">
         <v>86.86</v>
@@ -1905,7 +1905,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B135" s="3">
         <v>86.83</v>
@@ -1913,7 +1913,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B136" s="3">
         <v>86.68</v>

</xml_diff>